<commit_message>
adding mcisaac exp files, adding Jan full run fastq file, and adding modified bio/rnasample files for cbf1 expb
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_10.10.19.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_10.10.19.xlsx
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866094AA-15DA-014D-AC5D-54E3D3FCBCC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69FEBDC-5985-8F44-9EA5-2A3BB0572CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="460" windowWidth="24440" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -399,7 +409,7 @@
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="C22" sqref="C22:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -456,7 +466,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -503,7 +513,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -535,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -567,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -599,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -631,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -663,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -695,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -727,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -759,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -791,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -823,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -855,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -887,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -919,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -951,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -983,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1079,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1511,35 +1521,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C34" s="2"/>
       <c r="G34" s="4"/>
       <c r="H34" s="11"/>
       <c r="I34" s="12"/>
       <c r="J34" s="11"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C35" s="2"/>
       <c r="G35" s="4"/>
       <c r="H35" s="11"/>
       <c r="I35" s="12"/>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C36" s="2"/>
       <c r="G36" s="4"/>
       <c r="H36" s="11"/>
       <c r="I36" s="12"/>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C37" s="2"/>
       <c r="G37" s="4"/>
       <c r="H37" s="11"/>
       <c r="I37" s="12"/>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C38" s="2"/>
       <c r="G38" s="4"/>
       <c r="H38" s="11"/>
@@ -1547,7 +1557,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C39" s="2"/>
       <c r="G39" s="4"/>
       <c r="H39" s="11"/>
@@ -1555,7 +1565,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="6"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C40" s="2"/>
       <c r="G40" s="4"/>
       <c r="H40" s="11"/>
@@ -1563,7 +1573,7 @@
       <c r="J40" s="13"/>
       <c r="K40" s="6"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="C41" s="2"/>
       <c r="G41" s="4"/>
       <c r="H41" s="11"/>

</xml_diff>